<commit_message>
added : Notes des quiz et d'autres images dans /assets
</commit_message>
<xml_diff>
--- a/Premiere/Notes/Moyenne_des_notes_du_premier_trimestre.xlsx
+++ b/Premiere/Notes/Moyenne_des_notes_du_premier_trimestre.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26105"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CA2F60B-F01D-44BF-BD72-5A1EC7BDC91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E91B5E7-656D-4C09-929D-6D9CA70952D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,13 +33,13 @@
     <t xml:space="preserve">Noms et prénoms </t>
   </si>
   <si>
-    <t>Notes 1</t>
-  </si>
-  <si>
-    <t>Notes 2</t>
-  </si>
-  <si>
-    <t>Notes 3</t>
+    <t>Notes devoir-test octobre</t>
+  </si>
+  <si>
+    <t>Notes devoir-test chapitre 4</t>
+  </si>
+  <si>
+    <t>Notes d'examen trismestriel</t>
   </si>
   <si>
     <t>Moyenne</t>
@@ -426,16 +426,15 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="4" width="31.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75">

</xml_diff>